<commit_message>
UPdate how dwelling Stock is assigned
</commit_message>
<xml_diff>
--- a/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
+++ b/SuppXLS/Trades/ScenTrade__Trade_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\Trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D1CCBD-1535-46CB-A9EA-476C208DE296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7581D01-C883-4429-A33D-AD8CB13EB92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="14" r:id="rId1"/>
@@ -875,6 +875,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -884,7 +885,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{EE902F2F-0484-4915-A690-4EC96DD96FB2}"/>
@@ -2098,12 +2098,12 @@
       <c r="Z15" s="13"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="16"/>
@@ -2187,11 +2187,11 @@
       <c r="A19" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="22"/>
@@ -2219,11 +2219,11 @@
       <c r="A20" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="21"/>
       <c r="F20" s="21"/>
       <c r="G20" s="22"/>
@@ -2311,11 +2311,11 @@
       <c r="A23" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -2399,11 +2399,11 @@
       <c r="A26" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2519,11 +2519,11 @@
       <c r="A30" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="25"/>
       <c r="F30" s="25"/>
       <c r="G30" s="13"/>
@@ -2551,11 +2551,11 @@
       <c r="A31" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
       <c r="G31" s="13"/>
@@ -5276,8 +5276,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:N1304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1272" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1307" sqref="E1307"/>
+    <sheetView tabSelected="1" topLeftCell="A1263" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1250" sqref="H1250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7158,7 +7158,7 @@
       <c r="I54" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N54" s="33" t="s">
+      <c r="N54" s="30" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>